<commit_message>
Update `task-2` in `econometrics`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/econometrics/task-2/task-2.xlsx
+++ b/3-course-6-semester/econometrics/task-2/task-2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\egor\github\university\3-course-6-semester\econometrics\task-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59763CA4-58C8-44DE-9CE2-BEE37A313013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9590EA01-E2E0-4C60-A5C4-DB2100D9227F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E7C37711-55B5-4D4C-B546-27CE64F57E1C}"/>
+    <workbookView xWindow="-20610" yWindow="4560" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{E7C37711-55B5-4D4C-B546-27CE64F57E1C}"/>
   </bookViews>
   <sheets>
     <sheet name="ДЗ №2" sheetId="1" r:id="rId1"/>
+    <sheet name="Занятие №3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
   <si>
     <t>y</t>
   </si>
@@ -164,13 +165,116 @@
   </si>
   <si>
     <t>F (табл.) =</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x1 - число занятых (чел)</t>
+  </si>
+  <si>
+    <t>x2 - затраты на рекламу (тыс. руб.)</t>
+  </si>
+  <si>
+    <t>y - объём прод. (тыс. ед.)</t>
+  </si>
+  <si>
+    <t>R^2 =</t>
+  </si>
+  <si>
+    <t>Ryx1.x2^2</t>
+  </si>
+  <si>
+    <t>Ryx2.x1^2</t>
+  </si>
+  <si>
+    <t>Ryx1.x2</t>
+  </si>
+  <si>
+    <t>Ryx2.x1</t>
+  </si>
+  <si>
+    <t>Ryx1 = B1 + Rx1x2*B2</t>
+  </si>
+  <si>
+    <t>Ryx2 = Rx2x1*B1 + B2</t>
+  </si>
+  <si>
+    <t>d =</t>
+  </si>
+  <si>
+    <t>0,9586 = B1 + 0,7865 B2</t>
+  </si>
+  <si>
+    <t>0,95868745 = 0,7865 B1 + B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Доп. x1 </t>
+  </si>
+  <si>
+    <t>y'</t>
+  </si>
+  <si>
+    <t>x1'</t>
+  </si>
+  <si>
+    <t>x2'</t>
+  </si>
+  <si>
+    <t>y' = ln(y)</t>
+  </si>
+  <si>
+    <t>x1' = ln(x1)</t>
+  </si>
+  <si>
+    <t>x2' = ln(x2)</t>
+  </si>
+  <si>
+    <t>Предсказанное y'</t>
+  </si>
+  <si>
+    <t>СТЕПЕННАЯ РЕГРЕССИЯ</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>ДЗ</t>
+  </si>
+  <si>
+    <t>x1 - цена единицы товара (доллары)</t>
+  </si>
+  <si>
+    <t>y - объём продаж (млн. руб)</t>
+  </si>
+  <si>
+    <t>x2 - расходы на рекламу за пред. месяц</t>
+  </si>
+  <si>
+    <t>x3 - количество работников занятых сбытом</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,8 +317,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,8 +357,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -460,11 +584,124 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -480,16 +717,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -499,9 +730,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -522,12 +750,131 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1729,7 +2076,7 @@
             </a:rPr>
             <a:t>.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" i="1">
+          <a:endParaRPr lang="ru-RU" sz="1200" i="1" baseline="0">
             <a:latin typeface="+mj-lt"/>
           </a:endParaRPr>
         </a:p>
@@ -2023,8 +2370,8 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -2190,7 +2537,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -2317,6 +2664,81 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8243E845-094D-40B6-9273-1F55FB6EC0B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3219450" y="23021925"/>
+          <a:ext cx="3981450" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Найти уравнение регрессии</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> со значимыми параметрами</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2621,8 +3043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACBE7CC0-2A40-4A99-B552-5B4C7BB519A8}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,23 +3062,23 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="21"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="s">
@@ -2664,32 +3086,32 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15">
+      <c r="A5" s="13">
         <v>100</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="14">
         <v>9</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="13">
         <f>1/A5</f>
         <v>0.01</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="9">
         <v>200</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>6</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <f t="shared" ref="D6:D14" si="0">1/A6</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>6</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -2698,17 +3120,17 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="9">
         <v>300</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>5</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <f t="shared" si="0"/>
         <v>3.3333333333333335E-3</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -2719,17 +3141,17 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="9">
         <v>400</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>4</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>4</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -2740,17 +3162,17 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="A9" s="9">
         <v>500</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>3.7</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <v>3.7</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -2761,17 +3183,17 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="9">
         <v>600</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>3.6</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <f t="shared" si="0"/>
         <v>1.6666666666666668E-3</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <v>3.6</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -2782,17 +3204,17 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="9">
         <v>700</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>3.5</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <f t="shared" si="0"/>
         <v>1.4285714285714286E-3</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <v>3.5</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -2803,32 +3225,32 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="9">
         <v>150</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <v>6</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <f t="shared" si="0"/>
         <v>6.6666666666666671E-3</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
+      <c r="A13" s="9">
         <v>120</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>7</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="10">
         <v>7</v>
       </c>
       <c r="H13" t="s">
@@ -2836,17 +3258,17 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+      <c r="A14" s="11">
         <v>250</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="12">
         <v>3.5</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="11">
         <f t="shared" si="0"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="12">
         <v>3.5</v>
       </c>
       <c r="H14" s="3"/>
@@ -2887,10 +3309,10 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="19">
         <v>10</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -2951,13 +3373,13 @@
       </c>
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="23">
         <f>$I$20</f>
         <v>2.4688927280912001</v>
       </c>
@@ -2990,10 +3412,10 @@
       </c>
     </row>
     <row r="21" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="25">
         <f>$I$21</f>
         <v>592.2973260210365</v>
       </c>
@@ -3027,13 +3449,13 @@
     </row>
     <row r="22" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="27">
         <f>SQRT(1-$J$16/$J$17)</f>
         <v>0.94707558850407547</v>
       </c>
@@ -3098,13 +3520,13 @@
       <c r="J31" s="1">
         <v>5.0363956856208425E-2</v>
       </c>
-      <c r="L31" s="17" t="s">
+      <c r="L31" s="15" t="s">
         <v>40</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N31" s="8">
+      <c r="N31" s="7">
         <f>$F$23^2/(1-$F$23^2)*(($B$16-$I$15-1)/$I$15)</f>
         <v>69.633852420007059</v>
       </c>
@@ -3122,7 +3544,7 @@
       <c r="M32" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="N32" s="9">
+      <c r="N32" s="8">
         <f>_xlfn.F.INV.RT(0.05,1,8)</f>
         <v>5.3176550715787174</v>
       </c>
@@ -3161,13 +3583,13 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="29">
         <f>-$F$21/($F$20*AVERAGE(D5:D14)+$F$21)</f>
         <v>-0.99998127262422132</v>
       </c>
@@ -3199,4 +3621,1492 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3381694-2C74-4401-A1D7-2E8D71F6AA61}">
+  <dimension ref="B2:P127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="45"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="47"/>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="49"/>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="34">
+        <v>11</v>
+      </c>
+      <c r="C9" s="30">
+        <v>9</v>
+      </c>
+      <c r="D9" s="35">
+        <v>12</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="34">
+        <v>17</v>
+      </c>
+      <c r="C10" s="30">
+        <v>15</v>
+      </c>
+      <c r="D10" s="35">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.97825930555922225</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="34">
+        <v>15</v>
+      </c>
+      <c r="C11" s="30">
+        <v>13</v>
+      </c>
+      <c r="D11" s="35">
+        <v>21</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.95699126891321185</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="34">
+        <v>12</v>
+      </c>
+      <c r="C12" s="30">
+        <v>10</v>
+      </c>
+      <c r="D12" s="35">
+        <v>13</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.94470306003127236</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="34">
+        <v>13</v>
+      </c>
+      <c r="C13" s="30">
+        <v>11</v>
+      </c>
+      <c r="D13" s="35">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.75346881179356273</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="34">
+        <v>8</v>
+      </c>
+      <c r="C14" s="30">
+        <v>7</v>
+      </c>
+      <c r="D14" s="35">
+        <v>6</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="34">
+        <v>10</v>
+      </c>
+      <c r="C15" s="30">
+        <v>8</v>
+      </c>
+      <c r="D15" s="35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="34">
+        <v>14</v>
+      </c>
+      <c r="C16" s="30">
+        <v>13</v>
+      </c>
+      <c r="D16" s="35">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="34">
+        <v>16</v>
+      </c>
+      <c r="C17" s="30">
+        <v>15</v>
+      </c>
+      <c r="D17" s="35">
+        <v>22</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="36">
+        <v>18</v>
+      </c>
+      <c r="C18" s="37">
+        <v>20</v>
+      </c>
+      <c r="D18" s="38">
+        <v>18</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1">
+        <v>88.425993247580777</v>
+      </c>
+      <c r="K18" s="1">
+        <v>44.212996623790389</v>
+      </c>
+      <c r="L18" s="1">
+        <v>77.878824986426238</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1.6498642159698402E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="1">
+        <v>7</v>
+      </c>
+      <c r="J19" s="1">
+        <v>3.9740067524192222</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.56771525034560322</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="2">
+        <v>9</v>
+      </c>
+      <c r="J20" s="2">
+        <v>92.4</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="34">
+        <f>LN(B9)</f>
+        <v>2.3978952727983707</v>
+      </c>
+      <c r="C23" s="30">
+        <f>LN(C9)</f>
+        <v>2.1972245773362196</v>
+      </c>
+      <c r="D23" s="35">
+        <f>LN(D9)</f>
+        <v>2.4849066497880004</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3.8698494971349753</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.80991704527380326</v>
+      </c>
+      <c r="K23" s="1">
+        <v>4.7780813105701725</v>
+      </c>
+      <c r="L23" s="1">
+        <v>2.0167527821335807E-3</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1.9547000101021685</v>
+      </c>
+      <c r="N23" s="1">
+        <v>5.7849989841677818</v>
+      </c>
+      <c r="O23" s="1">
+        <v>1.9547000101021685</v>
+      </c>
+      <c r="P23" s="1">
+        <v>5.7849989841677818</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="34">
+        <f t="shared" ref="B24:D32" si="0">LN(B10)</f>
+        <v>2.8332133440562162</v>
+      </c>
+      <c r="C24" s="30">
+        <f t="shared" si="0"/>
+        <v>2.7080502011022101</v>
+      </c>
+      <c r="D24" s="35">
+        <f t="shared" si="0"/>
+        <v>2.9957322735539909</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.57921015716017976</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.10352519572221915</v>
+      </c>
+      <c r="K24" s="1">
+        <v>5.5948714041973693</v>
+      </c>
+      <c r="L24" s="1">
+        <v>8.2034275990532622E-4</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0.33441196870453072</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0.82400834561582881</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0.33441196870453072</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0.82400834561582881</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="34">
+        <f t="shared" si="0"/>
+        <v>2.7080502011022101</v>
+      </c>
+      <c r="C25" s="30">
+        <f t="shared" si="0"/>
+        <v>2.5649493574615367</v>
+      </c>
+      <c r="D25" s="35">
+        <f t="shared" si="0"/>
+        <v>3.044522437723423</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.17038564873154388</v>
+      </c>
+      <c r="J25" s="2">
+        <v>6.8463159303412124E-2</v>
+      </c>
+      <c r="K25" s="2">
+        <v>2.4887202177807191</v>
+      </c>
+      <c r="L25" s="2">
+        <v>4.167457697228192E-2</v>
+      </c>
+      <c r="M25" s="2">
+        <v>8.4960019020353661E-3</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0.3322752955610524</v>
+      </c>
+      <c r="O25" s="2">
+        <v>8.4960019020353661E-3</v>
+      </c>
+      <c r="P25" s="2">
+        <v>0.3322752955610524</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="34">
+        <f t="shared" si="0"/>
+        <v>2.4849066497880004</v>
+      </c>
+      <c r="C26" s="30">
+        <f t="shared" si="0"/>
+        <v>2.3025850929940459</v>
+      </c>
+      <c r="D26" s="35">
+        <f t="shared" si="0"/>
+        <v>2.5649493574615367</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="34">
+        <f t="shared" si="0"/>
+        <v>2.5649493574615367</v>
+      </c>
+      <c r="C27" s="30">
+        <f t="shared" si="0"/>
+        <v>2.3978952727983707</v>
+      </c>
+      <c r="D27" s="35">
+        <f t="shared" si="0"/>
+        <v>2.3025850929940459</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="34">
+        <f t="shared" si="0"/>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="C28" s="30">
+        <f t="shared" si="0"/>
+        <v>1.9459101490553132</v>
+      </c>
+      <c r="D28" s="35">
+        <f t="shared" si="0"/>
+        <v>1.791759469228055</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="34">
+        <f t="shared" si="0"/>
+        <v>2.3025850929940459</v>
+      </c>
+      <c r="C29" s="30">
+        <f t="shared" si="0"/>
+        <v>2.0794415416798357</v>
+      </c>
+      <c r="D29" s="35">
+        <f t="shared" si="0"/>
+        <v>1.9459101490553132</v>
+      </c>
+      <c r="H29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="34">
+        <f t="shared" si="0"/>
+        <v>2.6390573296152584</v>
+      </c>
+      <c r="C30" s="30">
+        <f t="shared" si="0"/>
+        <v>2.5649493574615367</v>
+      </c>
+      <c r="D30" s="35">
+        <f t="shared" si="0"/>
+        <v>2.9444389791664403</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="34">
+        <f t="shared" si="0"/>
+        <v>2.7725887222397811</v>
+      </c>
+      <c r="C31" s="30">
+        <f t="shared" si="0"/>
+        <v>2.7080502011022101</v>
+      </c>
+      <c r="D31" s="35">
+        <f t="shared" si="0"/>
+        <v>3.0910424533583161</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="36">
+        <f t="shared" si="0"/>
+        <v>2.8903717578961645</v>
+      </c>
+      <c r="C32" s="37">
+        <f t="shared" si="0"/>
+        <v>2.9957322735539909</v>
+      </c>
+      <c r="D32" s="38">
+        <f t="shared" si="0"/>
+        <v>2.8903717578961645</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
+        <v>11.12736869635512</v>
+      </c>
+      <c r="J32" s="1">
+        <v>-0.12736869635511994</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="1">
+        <v>2</v>
+      </c>
+      <c r="I33" s="1">
+        <v>15.965714829168549</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1.0342851708314509</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="45"/>
+      <c r="H34" s="1">
+        <v>3</v>
+      </c>
+      <c r="I34" s="1">
+        <v>14.977680163579734</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2.2319836420265915E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="47"/>
+      <c r="H35" s="1">
+        <v>4</v>
+      </c>
+      <c r="I35" s="1">
+        <v>11.876964502246842</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0.12303549775315759</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="49"/>
+      <c r="H36" s="1">
+        <v>5</v>
+      </c>
+      <c r="I36" s="1">
+        <v>11.94501771321239</v>
+      </c>
+      <c r="J36" s="1">
+        <v>1.0549822867876095</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H37" s="1">
+        <v>6</v>
+      </c>
+      <c r="I37" s="1">
+        <v>8.946634489645497</v>
+      </c>
+      <c r="J37" s="1">
+        <v>-0.94663448964549701</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H38" s="1">
+        <v>7</v>
+      </c>
+      <c r="I38" s="1">
+        <v>9.6962302955372213</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0.30376970446277873</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H39" s="1">
+        <v>8</v>
+      </c>
+      <c r="I39" s="1">
+        <v>14.636908866116645</v>
+      </c>
+      <c r="J39" s="1">
+        <v>-0.6369088661166451</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H40" s="1">
+        <v>9</v>
+      </c>
+      <c r="I40" s="1">
+        <v>16.306486126631636</v>
+      </c>
+      <c r="J40" s="1">
+        <v>-0.30648612663163632</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H41" s="2">
+        <v>10</v>
+      </c>
+      <c r="I41" s="2">
+        <v>18.520994317506361</v>
+      </c>
+      <c r="J41" s="2">
+        <v>-0.52099431750636072</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H46" s="3"/>
+      <c r="I46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0.95861168114177098</v>
+      </c>
+      <c r="K47" s="1">
+        <v>0.87445120565729095</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0.95861168114177131</v>
+      </c>
+      <c r="J48" s="1">
+        <v>1</v>
+      </c>
+      <c r="K48" s="1">
+        <v>0.78653612320470701</v>
+      </c>
+    </row>
+    <row r="49" spans="7:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H49" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I49" s="43">
+        <v>0.8744512056572914</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0.78653612320470689</v>
+      </c>
+      <c r="K49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <f>MDETERM(I47:K49)</f>
+        <v>1.6401849551797038E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <f>MDETERM(J48:K49)</f>
+        <v>0.38136092689411005</v>
+      </c>
+    </row>
+    <row r="54" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>48</v>
+      </c>
+      <c r="H54">
+        <f>1-(H52/H53)</f>
+        <v>0.95699126891321185</v>
+      </c>
+    </row>
+    <row r="57" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>49</v>
+      </c>
+      <c r="H57">
+        <f>1-((1-I11)/(1-I49^2))</f>
+        <v>0.81724471568035295</v>
+      </c>
+      <c r="I57" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="J57">
+        <f>H57^0.5</f>
+        <v>0.90401588242704722</v>
+      </c>
+    </row>
+    <row r="58" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>50</v>
+      </c>
+      <c r="H58">
+        <f>1-((1-I11)/(1-I48^2))</f>
+        <v>0.46944488858993227</v>
+      </c>
+      <c r="I58" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="J58">
+        <f>H58^0.5</f>
+        <v>0.68516048382107697</v>
+      </c>
+    </row>
+    <row r="61" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>53</v>
+      </c>
+      <c r="I61" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>54</v>
+      </c>
+      <c r="I62" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>55</v>
+      </c>
+      <c r="H65">
+        <f>H53</f>
+        <v>0.38136092689411005</v>
+      </c>
+    </row>
+    <row r="67" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <f>0.579*12.1/13.4</f>
+        <v>0.52282835820895512</v>
+      </c>
+    </row>
+    <row r="69" spans="7:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H70" s="41"/>
+      <c r="I70" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="J70" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="K70" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="L70" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="M70" s="41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I71" s="1">
+        <v>2</v>
+      </c>
+      <c r="J71" s="1">
+        <v>88.425993247580777</v>
+      </c>
+      <c r="K71" s="1">
+        <v>44.212996623790389</v>
+      </c>
+      <c r="L71" s="1">
+        <v>77.878824986426238</v>
+      </c>
+      <c r="M71" s="1">
+        <v>1.6498642159698402E-5</v>
+      </c>
+    </row>
+    <row r="72" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>44</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72" s="42">
+        <f>I49^2*J75</f>
+        <v>70.65503778337532</v>
+      </c>
+      <c r="K72">
+        <f>J72/I72</f>
+        <v>70.65503778337532</v>
+      </c>
+      <c r="L72">
+        <f>K72/K74</f>
+        <v>124.45506394334704</v>
+      </c>
+      <c r="M72" s="1"/>
+    </row>
+    <row r="73" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>58</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="J73" s="42">
+        <f>J71-J72</f>
+        <v>17.770955464205457</v>
+      </c>
+      <c r="K73">
+        <f>J73/I73</f>
+        <v>17.770955464205457</v>
+      </c>
+      <c r="L73">
+        <f>K73/K74</f>
+        <v>31.302586029505431</v>
+      </c>
+      <c r="M73" s="1"/>
+    </row>
+    <row r="74" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I74" s="1">
+        <v>7</v>
+      </c>
+      <c r="J74" s="1">
+        <v>3.9740067524192222</v>
+      </c>
+      <c r="K74" s="1">
+        <v>0.56771525034560322</v>
+      </c>
+      <c r="L74" s="1"/>
+      <c r="M74" s="40"/>
+    </row>
+    <row r="75" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I75" s="1">
+        <v>9</v>
+      </c>
+      <c r="J75" s="1">
+        <v>92.4</v>
+      </c>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+    </row>
+    <row r="80" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H83" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I83" s="4"/>
+    </row>
+    <row r="84" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H84" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I84" s="1">
+        <v>0.98251582274718685</v>
+      </c>
+    </row>
+    <row r="85" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I85" s="1">
+        <v>0.96533734194858156</v>
+      </c>
+    </row>
+    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I86" s="1">
+        <v>0.95543372536246196</v>
+      </c>
+    </row>
+    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H87" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I87" s="1">
+        <v>5.3856973046439008E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H88" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I88" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H90" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H91" s="3"/>
+      <c r="I91" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L91" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M91" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I92" s="1">
+        <v>2</v>
+      </c>
+      <c r="J92" s="1">
+        <v>0.56545645369203956</v>
+      </c>
+      <c r="K92" s="1">
+        <v>0.28272822684601978</v>
+      </c>
+      <c r="L92" s="1">
+        <v>97.473214310573709</v>
+      </c>
+      <c r="M92" s="1">
+        <v>7.7538343730010616E-6</v>
+      </c>
+    </row>
+    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H93" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I93" s="1">
+        <v>7</v>
+      </c>
+      <c r="J93" s="1">
+        <v>2.0304014820074007E-2</v>
+      </c>
+      <c r="K93" s="1">
+        <v>2.9005735457248581E-3</v>
+      </c>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+    </row>
+    <row r="94" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H94" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I94" s="2">
+        <v>9</v>
+      </c>
+      <c r="J94" s="2">
+        <v>0.58576046851211361</v>
+      </c>
+      <c r="K94" s="2"/>
+      <c r="L94" s="2"/>
+      <c r="M94" s="2"/>
+    </row>
+    <row r="95" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H96" s="3"/>
+      <c r="I96" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K96" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L96" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M96" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N96" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O96" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P96" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E97" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="F97" s="54">
+        <f>EXP(I97)</f>
+        <v>2.1172578384222343</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I97" s="1">
+        <v>0.75012177898404153</v>
+      </c>
+      <c r="J97" s="1">
+        <v>0.14173722977822362</v>
+      </c>
+      <c r="K97" s="1">
+        <v>5.2923411876876516</v>
+      </c>
+      <c r="L97" s="1">
+        <v>1.1327505372360545E-3</v>
+      </c>
+      <c r="M97" s="1">
+        <v>0.41496648809687492</v>
+      </c>
+      <c r="N97" s="1">
+        <v>1.0852770698712082</v>
+      </c>
+      <c r="O97" s="1">
+        <v>0.41496648809687492</v>
+      </c>
+      <c r="P97" s="1">
+        <v>1.0852770698712082</v>
+      </c>
+    </row>
+    <row r="98" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E98" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="F98" s="56">
+        <f>I98</f>
+        <v>0.59220566333891078</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I98" s="1">
+        <v>0.59220566333891078</v>
+      </c>
+      <c r="J98" s="1">
+        <v>0.11057766148667508</v>
+      </c>
+      <c r="K98" s="1">
+        <v>5.3555632790287682</v>
+      </c>
+      <c r="L98" s="1">
+        <v>1.05783511226906E-3</v>
+      </c>
+      <c r="M98" s="1">
+        <v>0.33073104330310138</v>
+      </c>
+      <c r="N98" s="1">
+        <v>0.85368028337472013</v>
+      </c>
+      <c r="O98" s="1">
+        <v>0.33073104330310138</v>
+      </c>
+      <c r="P98" s="1">
+        <v>0.85368028337472013</v>
+      </c>
+    </row>
+    <row r="99" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E99" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="F99" s="58">
+        <f>I99</f>
+        <v>0.14137337090079588</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I99" s="2">
+        <v>0.14137337090079588</v>
+      </c>
+      <c r="J99" s="2">
+        <v>7.6033169676370069E-2</v>
+      </c>
+      <c r="K99" s="2">
+        <v>1.8593644261122069</v>
+      </c>
+      <c r="L99" s="2">
+        <v>0.10530968717050911</v>
+      </c>
+      <c r="M99" s="2">
+        <v>-3.8416506041417914E-2</v>
+      </c>
+      <c r="N99" s="2">
+        <v>0.32116324784300965</v>
+      </c>
+      <c r="O99" s="2">
+        <v>-3.8416506041417914E-2</v>
+      </c>
+      <c r="P99" s="2">
+        <v>0.32116324784300965</v>
+      </c>
+    </row>
+    <row r="103" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="H103" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="H105" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="H106" s="1">
+        <v>1</v>
+      </c>
+      <c r="I106" s="1">
+        <v>2.4026302467643283</v>
+      </c>
+      <c r="J106" s="1">
+        <v>-4.7349739659576784E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="H107" s="1">
+        <v>2</v>
+      </c>
+      <c r="I107" s="1">
+        <v>2.7773612145114797</v>
+      </c>
+      <c r="J107" s="1">
+        <v>5.5852129544736506E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="H108" s="1">
+        <v>3</v>
+      </c>
+      <c r="I108" s="1">
+        <v>2.6995137144543326</v>
+      </c>
+      <c r="J108" s="1">
+        <v>8.5364866478774282E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="H109" s="1">
+        <v>4</v>
+      </c>
+      <c r="I109" s="1">
+        <v>2.4763412482290361</v>
+      </c>
+      <c r="J109" s="1">
+        <v>8.5654015589642363E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="H110" s="1">
+        <v>5</v>
+      </c>
+      <c r="I110" s="1">
+        <v>2.4956931560113298</v>
+      </c>
+      <c r="J110" s="1">
+        <v>6.9256201450206945E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="H111" s="1">
+        <v>6</v>
+      </c>
+      <c r="I111" s="1">
+        <v>2.155807865611453</v>
+      </c>
+      <c r="J111" s="1">
+        <v>-7.6366323931617242E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H112" s="1">
+        <v>7</v>
+      </c>
+      <c r="I112" s="1">
+        <v>2.2566787137910556</v>
+      </c>
+      <c r="J112" s="1">
+        <v>4.5906379202990344E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B113" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C113" s="50"/>
+      <c r="D113" s="50"/>
+      <c r="E113" s="50"/>
+      <c r="F113" s="45"/>
+      <c r="H113" s="1">
+        <v>8</v>
+      </c>
+      <c r="I113" s="1">
+        <v>2.6853645785467219</v>
+      </c>
+      <c r="J113" s="1">
+        <v>-4.630724893146354E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B114" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C114" s="51"/>
+      <c r="D114" s="51"/>
+      <c r="E114" s="51"/>
+      <c r="F114" s="47"/>
+      <c r="H114" s="1">
+        <v>9</v>
+      </c>
+      <c r="I114" s="1">
+        <v>2.7908355359115777</v>
+      </c>
+      <c r="J114" s="1">
+        <v>-1.8246813671796591E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C115" s="51"/>
+      <c r="D115" s="51"/>
+      <c r="E115" s="51"/>
+      <c r="F115" s="47"/>
+      <c r="H115" s="2">
+        <v>10</v>
+      </c>
+      <c r="I115" s="2">
+        <v>2.9328329958001058</v>
+      </c>
+      <c r="J115" s="2">
+        <v>-4.2461237903941296E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C116" s="52"/>
+      <c r="D116" s="52"/>
+      <c r="E116" s="52"/>
+      <c r="F116" s="49"/>
+    </row>
+    <row r="117" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C118" s="60"/>
+      <c r="D118" s="60"/>
+      <c r="E118" s="61"/>
+    </row>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B119" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C119" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D119" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E119" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="120" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B120" s="34">
+        <v>4</v>
+      </c>
+      <c r="C120" s="30">
+        <v>1</v>
+      </c>
+      <c r="D120" s="30">
+        <v>8</v>
+      </c>
+      <c r="E120" s="35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B121" s="34">
+        <v>5.2</v>
+      </c>
+      <c r="C121" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="D121" s="30">
+        <v>9</v>
+      </c>
+      <c r="E121" s="35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="122" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B122" s="34">
+        <v>3.8</v>
+      </c>
+      <c r="C122" s="30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D122" s="30">
+        <v>6</v>
+      </c>
+      <c r="E122" s="35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B123" s="34">
+        <v>2.9</v>
+      </c>
+      <c r="C123" s="30">
+        <v>1.2</v>
+      </c>
+      <c r="D123" s="30">
+        <v>5</v>
+      </c>
+      <c r="E123" s="35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B124" s="34">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C124" s="30">
+        <v>0.95</v>
+      </c>
+      <c r="D124" s="30">
+        <v>7</v>
+      </c>
+      <c r="E124" s="35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B125" s="34">
+        <v>4.5</v>
+      </c>
+      <c r="C125" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="D125" s="30">
+        <v>6</v>
+      </c>
+      <c r="E125" s="35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="126" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B126" s="34">
+        <v>3.7</v>
+      </c>
+      <c r="C126" s="30">
+        <v>1</v>
+      </c>
+      <c r="D126" s="30">
+        <v>6</v>
+      </c>
+      <c r="E126" s="35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="127" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B127" s="36">
+        <v>5</v>
+      </c>
+      <c r="C127" s="37">
+        <v>0.95</v>
+      </c>
+      <c r="D127" s="37">
+        <v>10</v>
+      </c>
+      <c r="E127" s="38">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B118:E118"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>